<commit_message>
Conduct S4 tests for REST and REST with one endpoint
</commit_message>
<xml_diff>
--- a/Wyniki 3/S4.xlsx
+++ b/Wyniki 3/S4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kacpe\OneDrive\Pulpit\Projekty\Praca magisterska\Wyniki 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D326C29E-D04D-4F3C-AFD5-0D975A73FE92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A201F5-7265-44B5-A38A-CCA6FF090F8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25710" yWindow="-2340" windowWidth="25820" windowHeight="15500" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REST" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="57">
   <si>
     <t>Maksymalna liczba użytkowników</t>
   </si>
@@ -138,6 +138,81 @@
   </si>
   <si>
     <t>840MB</t>
+  </si>
+  <si>
+    <t>Średni czas grupy (ms)</t>
+  </si>
+  <si>
+    <t>Maksymalny czas grupy (ms)</t>
+  </si>
+  <si>
+    <t>62MB</t>
+  </si>
+  <si>
+    <t>332MB</t>
+  </si>
+  <si>
+    <t>p(90) grupy (ms)</t>
+  </si>
+  <si>
+    <t>p(95) grupy (ms)</t>
+  </si>
+  <si>
+    <t>1,6GB</t>
+  </si>
+  <si>
+    <t>303MB</t>
+  </si>
+  <si>
+    <t>297MB</t>
+  </si>
+  <si>
+    <t>298MB</t>
+  </si>
+  <si>
+    <t>1,7GB</t>
+  </si>
+  <si>
+    <t>307MB</t>
+  </si>
+  <si>
+    <t>308MB</t>
+  </si>
+  <si>
+    <t>311MB</t>
+  </si>
+  <si>
+    <t>305MB</t>
+  </si>
+  <si>
+    <t>309MB</t>
+  </si>
+  <si>
+    <t>203MB</t>
+  </si>
+  <si>
+    <t>9MB</t>
+  </si>
+  <si>
+    <t>2GB</t>
+  </si>
+  <si>
+    <t>90MB</t>
+  </si>
+  <si>
+    <t>3,2GB</t>
+  </si>
+  <si>
+    <t>140MB</t>
+  </si>
+  <si>
+    <t>3,1GB</t>
+  </si>
+  <si>
+    <t>139MB</t>
+  </si>
+  <si>
+    <t>143MB</t>
   </si>
 </sst>
 </file>
@@ -821,8 +896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="E7:L50"/>
   <sheetViews>
-    <sheetView topLeftCell="D13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView topLeftCell="D30" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -832,7 +907,7 @@
     <col min="7" max="11" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E7" s="3" t="s">
         <v>12</v>
       </c>
@@ -843,7 +918,7 @@
       <c r="J7" s="4"/>
       <c r="K7" s="5"/>
     </row>
-    <row r="8" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E8" s="1" t="s">
         <v>0</v>
       </c>
@@ -866,120 +941,256 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E9" s="6">
         <v>100</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-    </row>
-    <row r="10" spans="5:11" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="G9" s="1">
+        <v>8.94</v>
+      </c>
+      <c r="H9" s="1">
+        <v>8.9</v>
+      </c>
+      <c r="I9" s="1">
+        <v>8.84</v>
+      </c>
+      <c r="J9" s="1">
+        <v>9</v>
+      </c>
+      <c r="K9" s="1">
+        <v>9.26</v>
+      </c>
+      <c r="L9">
+        <f>AVERAGE(G9:K9)</f>
+        <v>8.9879999999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E10" s="7"/>
       <c r="F10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-    </row>
-    <row r="11" spans="5:11" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="G10" s="1">
+        <v>164.21</v>
+      </c>
+      <c r="H10" s="1">
+        <v>156</v>
+      </c>
+      <c r="I10" s="1">
+        <v>157.57</v>
+      </c>
+      <c r="J10" s="1">
+        <v>161.34</v>
+      </c>
+      <c r="K10" s="1">
+        <v>152.1</v>
+      </c>
+      <c r="L10">
+        <f t="shared" ref="L10:L50" si="0">AVERAGE(G10:K10)</f>
+        <v>158.244</v>
+      </c>
+    </row>
+    <row r="11" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E11" s="7"/>
       <c r="F11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-    </row>
-    <row r="12" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="G11" s="1">
+        <v>14.71</v>
+      </c>
+      <c r="H11" s="1">
+        <v>14.07</v>
+      </c>
+      <c r="I11" s="1">
+        <v>14.77</v>
+      </c>
+      <c r="J11" s="1">
+        <v>14.47</v>
+      </c>
+      <c r="K11" s="1">
+        <v>15.18</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>14.639999999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E12" s="7"/>
       <c r="F12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-    </row>
-    <row r="13" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="G12" s="1">
+        <v>17.07</v>
+      </c>
+      <c r="H12" s="1">
+        <v>16.34</v>
+      </c>
+      <c r="I12" s="1">
+        <v>17.12</v>
+      </c>
+      <c r="J12" s="1">
+        <v>16.5</v>
+      </c>
+      <c r="K12" s="1">
+        <v>17.53</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>16.911999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E13" s="7"/>
       <c r="F13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-    </row>
-    <row r="14" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="G13" s="1">
+        <v>1.07</v>
+      </c>
+      <c r="H13" s="1">
+        <v>1.06</v>
+      </c>
+      <c r="I13" s="1">
+        <v>1.06</v>
+      </c>
+      <c r="J13" s="1">
+        <v>1.08</v>
+      </c>
+      <c r="K13" s="1">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>1.0760000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E14" s="7"/>
       <c r="F14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-    </row>
-    <row r="15" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="G14" s="1">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0</v>
+      </c>
+      <c r="K14" s="1">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E15" s="7"/>
       <c r="F15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-    </row>
-    <row r="16" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="G15" s="1">
+        <v>148.38999999999999</v>
+      </c>
+      <c r="H15" s="1">
+        <v>149.86000000000001</v>
+      </c>
+      <c r="I15" s="1">
+        <v>153.15</v>
+      </c>
+      <c r="J15" s="1">
+        <v>149.07</v>
+      </c>
+      <c r="K15" s="1">
+        <v>142.19999999999999</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>148.53400000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E16" s="7"/>
       <c r="F16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
+      <c r="G16" s="1">
+        <v>1.97</v>
+      </c>
+      <c r="H16" s="1">
+        <v>1.87</v>
+      </c>
+      <c r="I16" s="1">
+        <v>1.94</v>
+      </c>
+      <c r="J16" s="1">
+        <v>1.91</v>
+      </c>
+      <c r="K16" s="1">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>1.9439999999999997</v>
+      </c>
     </row>
     <row r="17" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E17" s="7"/>
       <c r="F17" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
+      <c r="G17" s="1">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="H17" s="1">
+        <v>2.17</v>
+      </c>
+      <c r="I17" s="1">
+        <v>2.27</v>
+      </c>
+      <c r="J17" s="1">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="K17" s="1">
+        <v>2.34</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="0"/>
+        <v>2.2559999999999998</v>
+      </c>
     </row>
     <row r="18" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E18" s="7"/>
       <c r="F18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" t="e">
-        <f>AVERAGE(G18:K18)</f>
-        <v>#DIV/0!</v>
+      <c r="G18" s="1">
+        <v>666688</v>
+      </c>
+      <c r="H18" s="1">
+        <v>666736</v>
+      </c>
+      <c r="I18" s="1">
+        <v>666736</v>
+      </c>
+      <c r="J18" s="1">
+        <v>666648</v>
+      </c>
+      <c r="K18" s="1">
+        <v>666496</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="0"/>
+        <v>666660.80000000005</v>
       </c>
     </row>
     <row r="19" spans="5:12" x14ac:dyDescent="0.25">
@@ -987,14 +1198,24 @@
       <c r="F19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" t="e">
-        <f t="shared" ref="L19:L50" si="0">AVERAGE(G19:K19)</f>
-        <v>#DIV/0!</v>
+      <c r="G19" s="1">
+        <v>960.7</v>
+      </c>
+      <c r="H19" s="1">
+        <v>960.7</v>
+      </c>
+      <c r="I19" s="1">
+        <v>960.1</v>
+      </c>
+      <c r="J19" s="1">
+        <v>960.8</v>
+      </c>
+      <c r="K19" s="1">
+        <v>960.1</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="0"/>
+        <v>960.48000000000013</v>
       </c>
     </row>
     <row r="20" spans="5:12" x14ac:dyDescent="0.25">
@@ -1002,14 +1223,24 @@
       <c r="F20" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="G20" s="1">
+        <v>693.98</v>
+      </c>
+      <c r="H20" s="1">
+        <v>693.98</v>
+      </c>
+      <c r="I20" s="1">
+        <v>694.47</v>
+      </c>
+      <c r="J20" s="1">
+        <v>693.84</v>
+      </c>
+      <c r="K20" s="1">
+        <v>694.19</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="0"/>
+        <v>694.0920000000001</v>
       </c>
     </row>
     <row r="21" spans="5:12" x14ac:dyDescent="0.25">
@@ -1017,11 +1248,21 @@
       <c r="F21" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
+      <c r="G21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="L21" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -1032,11 +1273,21 @@
       <c r="F22" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
+      <c r="G22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="L22" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -1047,61 +1298,101 @@
         <v>1000</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>32</v>
+      </c>
+      <c r="G23" s="2">
+        <v>1040</v>
+      </c>
+      <c r="H23" s="2">
+        <v>1050</v>
+      </c>
+      <c r="I23" s="2">
+        <v>1080</v>
+      </c>
+      <c r="J23" s="2">
+        <v>1080</v>
+      </c>
+      <c r="K23" s="2">
+        <v>1080</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="0"/>
+        <v>1066</v>
       </c>
     </row>
     <row r="24" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E24" s="7"/>
       <c r="F24" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>33</v>
+      </c>
+      <c r="G24" s="2">
+        <v>1380</v>
+      </c>
+      <c r="H24" s="2">
+        <v>1580</v>
+      </c>
+      <c r="I24" s="2">
+        <v>1400</v>
+      </c>
+      <c r="J24" s="2">
+        <v>1380</v>
+      </c>
+      <c r="K24" s="2">
+        <v>1710</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="0"/>
+        <v>1490</v>
       </c>
     </row>
     <row r="25" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E25" s="7"/>
       <c r="F25" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-      <c r="L25" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>36</v>
+      </c>
+      <c r="G25" s="2">
+        <v>1240</v>
+      </c>
+      <c r="H25" s="2">
+        <v>1250</v>
+      </c>
+      <c r="I25" s="2">
+        <v>1290</v>
+      </c>
+      <c r="J25" s="2">
+        <v>1290</v>
+      </c>
+      <c r="K25" s="2">
+        <v>1290</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="0"/>
+        <v>1272</v>
       </c>
     </row>
     <row r="26" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E26" s="7"/>
       <c r="F26" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-      <c r="L26" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>37</v>
+      </c>
+      <c r="G26" s="2">
+        <v>1250</v>
+      </c>
+      <c r="H26" s="2">
+        <v>1260</v>
+      </c>
+      <c r="I26" s="2">
+        <v>1300</v>
+      </c>
+      <c r="J26" s="2">
+        <v>1300</v>
+      </c>
+      <c r="K26" s="2">
+        <v>1310</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="0"/>
+        <v>1284</v>
       </c>
     </row>
     <row r="27" spans="5:12" x14ac:dyDescent="0.25">
@@ -1109,14 +1400,24 @@
       <c r="F27" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="G27" s="2">
+        <v>131.08000000000001</v>
+      </c>
+      <c r="H27" s="2">
+        <v>131.25</v>
+      </c>
+      <c r="I27" s="2">
+        <v>136.05000000000001</v>
+      </c>
+      <c r="J27" s="2">
+        <v>135.91</v>
+      </c>
+      <c r="K27" s="2">
+        <v>135.22</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="0"/>
+        <v>133.90200000000002</v>
       </c>
     </row>
     <row r="28" spans="5:12" x14ac:dyDescent="0.25">
@@ -1124,14 +1425,24 @@
       <c r="F28" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="G28" s="2">
+        <v>0</v>
+      </c>
+      <c r="H28" s="2">
+        <v>0</v>
+      </c>
+      <c r="I28" s="2">
+        <v>0</v>
+      </c>
+      <c r="J28" s="2">
+        <v>0</v>
+      </c>
+      <c r="K28" s="2">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="5:12" x14ac:dyDescent="0.25">
@@ -1139,14 +1450,24 @@
       <c r="F29" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
-      <c r="L29" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="G29" s="2">
+        <v>214.96</v>
+      </c>
+      <c r="H29" s="2">
+        <v>253.16</v>
+      </c>
+      <c r="I29" s="2">
+        <v>217.28</v>
+      </c>
+      <c r="J29" s="2">
+        <v>211.29</v>
+      </c>
+      <c r="K29" s="2">
+        <v>261.25</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="0"/>
+        <v>231.58800000000002</v>
       </c>
     </row>
     <row r="30" spans="5:12" x14ac:dyDescent="0.25">
@@ -1154,14 +1475,24 @@
       <c r="F30" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-      <c r="L30" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="G30" s="2">
+        <v>158.24</v>
+      </c>
+      <c r="H30" s="2">
+        <v>159.16999999999999</v>
+      </c>
+      <c r="I30" s="2">
+        <v>164.48</v>
+      </c>
+      <c r="J30" s="2">
+        <v>164.16</v>
+      </c>
+      <c r="K30" s="2">
+        <v>164.52</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="0"/>
+        <v>162.11399999999998</v>
       </c>
     </row>
     <row r="31" spans="5:12" x14ac:dyDescent="0.25">
@@ -1169,14 +1500,24 @@
       <c r="F31" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="G31" s="2">
+        <v>160.97999999999999</v>
+      </c>
+      <c r="H31" s="2">
+        <v>162.57</v>
+      </c>
+      <c r="I31" s="2">
+        <v>167.31</v>
+      </c>
+      <c r="J31" s="2">
+        <v>166.95</v>
+      </c>
+      <c r="K31" s="2">
+        <v>168.47</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="0"/>
+        <v>165.256</v>
       </c>
     </row>
     <row r="32" spans="5:12" x14ac:dyDescent="0.25">
@@ -1184,14 +1525,24 @@
       <c r="F32" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-      <c r="L32" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="G32" s="2">
+        <v>3281848</v>
+      </c>
+      <c r="H32" s="2">
+        <v>3279744</v>
+      </c>
+      <c r="I32" s="2">
+        <v>3219424</v>
+      </c>
+      <c r="J32" s="2">
+        <v>3221088</v>
+      </c>
+      <c r="K32" s="2">
+        <v>3229592</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="0"/>
+        <v>3246339.2</v>
       </c>
     </row>
     <row r="33" spans="5:12" x14ac:dyDescent="0.25">
@@ -1199,14 +1550,24 @@
       <c r="F33" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-      <c r="L33" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="G33" s="2">
+        <v>960.6</v>
+      </c>
+      <c r="H33" s="2">
+        <v>960.6</v>
+      </c>
+      <c r="I33" s="2">
+        <v>960.7</v>
+      </c>
+      <c r="J33" s="2">
+        <v>960.7</v>
+      </c>
+      <c r="K33" s="2">
+        <v>960.5</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="0"/>
+        <v>960.62000000000012</v>
       </c>
     </row>
     <row r="34" spans="5:12" x14ac:dyDescent="0.25">
@@ -1214,14 +1575,24 @@
       <c r="F34" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
-      <c r="L34" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="G34" s="2">
+        <v>3416.4</v>
+      </c>
+      <c r="H34" s="2">
+        <v>3414.16</v>
+      </c>
+      <c r="I34" s="2">
+        <v>3351.07</v>
+      </c>
+      <c r="J34" s="2">
+        <v>3352.9</v>
+      </c>
+      <c r="K34" s="2">
+        <v>3362.3</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="0"/>
+        <v>3379.3659999999995</v>
       </c>
     </row>
     <row r="35" spans="5:12" x14ac:dyDescent="0.25">
@@ -1229,11 +1600,21 @@
       <c r="F35" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
+      <c r="G35" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="L35" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -1244,11 +1625,21 @@
       <c r="F36" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
+      <c r="G36" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="L36" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -1259,61 +1650,101 @@
         <v>4000</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
-      <c r="L37" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>32</v>
+      </c>
+      <c r="G37" s="1">
+        <v>7120</v>
+      </c>
+      <c r="H37" s="1">
+        <v>7090</v>
+      </c>
+      <c r="I37" s="1">
+        <v>7010</v>
+      </c>
+      <c r="J37" s="1">
+        <v>7150</v>
+      </c>
+      <c r="K37" s="1">
+        <v>7060</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="0"/>
+        <v>7086</v>
       </c>
     </row>
     <row r="38" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E38" s="7"/>
       <c r="F38" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="1"/>
-      <c r="L38" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>33</v>
+      </c>
+      <c r="G38" s="1">
+        <v>8500</v>
+      </c>
+      <c r="H38" s="1">
+        <v>8370</v>
+      </c>
+      <c r="I38" s="1">
+        <v>8370</v>
+      </c>
+      <c r="J38" s="1">
+        <v>8580</v>
+      </c>
+      <c r="K38" s="1">
+        <v>8400</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="0"/>
+        <v>8444</v>
       </c>
     </row>
     <row r="39" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E39" s="7"/>
       <c r="F39" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-      <c r="K39" s="1"/>
-      <c r="L39" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>36</v>
+      </c>
+      <c r="G39" s="1">
+        <v>8190</v>
+      </c>
+      <c r="H39" s="1">
+        <v>8150</v>
+      </c>
+      <c r="I39" s="1">
+        <v>8060</v>
+      </c>
+      <c r="J39" s="1">
+        <v>8230</v>
+      </c>
+      <c r="K39" s="1">
+        <v>8110</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="0"/>
+        <v>8148</v>
       </c>
     </row>
     <row r="40" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E40" s="7"/>
       <c r="F40" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
-      <c r="K40" s="1"/>
-      <c r="L40" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>37</v>
+      </c>
+      <c r="G40" s="1">
+        <v>8210</v>
+      </c>
+      <c r="H40" s="1">
+        <v>8160</v>
+      </c>
+      <c r="I40" s="1">
+        <v>8080</v>
+      </c>
+      <c r="J40" s="1">
+        <v>8250</v>
+      </c>
+      <c r="K40" s="1">
+        <v>8130</v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="0"/>
+        <v>8166</v>
       </c>
     </row>
     <row r="41" spans="5:12" x14ac:dyDescent="0.25">
@@ -1321,14 +1752,24 @@
       <c r="F41" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
-      <c r="K41" s="1"/>
-      <c r="L41" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="G41" s="1">
+        <v>890.47</v>
+      </c>
+      <c r="H41" s="1">
+        <v>886.61</v>
+      </c>
+      <c r="I41" s="1">
+        <v>877.06</v>
+      </c>
+      <c r="J41" s="1">
+        <v>894.35</v>
+      </c>
+      <c r="K41" s="1">
+        <v>883.19</v>
+      </c>
+      <c r="L41">
+        <f t="shared" si="0"/>
+        <v>886.33600000000001</v>
       </c>
     </row>
     <row r="42" spans="5:12" x14ac:dyDescent="0.25">
@@ -1336,14 +1777,24 @@
       <c r="F42" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
-      <c r="K42" s="1"/>
-      <c r="L42" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="G42" s="1">
+        <v>0</v>
+      </c>
+      <c r="H42" s="1">
+        <v>0</v>
+      </c>
+      <c r="I42" s="1">
+        <v>0</v>
+      </c>
+      <c r="J42" s="1">
+        <v>0</v>
+      </c>
+      <c r="K42" s="1">
+        <v>0</v>
+      </c>
+      <c r="L42">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="5:12" x14ac:dyDescent="0.25">
@@ -1351,14 +1802,24 @@
       <c r="F43" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
-      <c r="J43" s="1"/>
-      <c r="K43" s="1"/>
-      <c r="L43" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="G43" s="1">
+        <v>1240</v>
+      </c>
+      <c r="H43" s="1">
+        <v>1150</v>
+      </c>
+      <c r="I43" s="1">
+        <v>1170</v>
+      </c>
+      <c r="J43" s="1">
+        <v>1280</v>
+      </c>
+      <c r="K43" s="1">
+        <v>1200</v>
+      </c>
+      <c r="L43">
+        <f t="shared" si="0"/>
+        <v>1208</v>
       </c>
     </row>
     <row r="44" spans="5:12" x14ac:dyDescent="0.25">
@@ -1366,14 +1827,24 @@
       <c r="F44" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
-      <c r="K44" s="1"/>
-      <c r="L44" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="G44" s="1">
+        <v>1030</v>
+      </c>
+      <c r="H44" s="1">
+        <v>1030</v>
+      </c>
+      <c r="I44" s="1">
+        <v>1010</v>
+      </c>
+      <c r="J44" s="1">
+        <v>1040</v>
+      </c>
+      <c r="K44" s="1">
+        <v>1020</v>
+      </c>
+      <c r="L44">
+        <f t="shared" si="0"/>
+        <v>1026</v>
       </c>
     </row>
     <row r="45" spans="5:12" x14ac:dyDescent="0.25">
@@ -1381,14 +1852,24 @@
       <c r="F45" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
-      <c r="I45" s="1"/>
-      <c r="J45" s="1"/>
-      <c r="K45" s="1"/>
-      <c r="L45" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="G45" s="1">
+        <v>1040</v>
+      </c>
+      <c r="H45" s="1">
+        <v>1030</v>
+      </c>
+      <c r="I45" s="1">
+        <v>1020</v>
+      </c>
+      <c r="J45" s="1">
+        <v>1040</v>
+      </c>
+      <c r="K45" s="1">
+        <v>1030</v>
+      </c>
+      <c r="L45">
+        <f t="shared" si="0"/>
+        <v>1032</v>
       </c>
     </row>
     <row r="46" spans="5:12" x14ac:dyDescent="0.25">
@@ -1396,14 +1877,24 @@
       <c r="F46" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
-      <c r="I46" s="1"/>
-      <c r="J46" s="1"/>
-      <c r="K46" s="1"/>
-      <c r="L46" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="G46" s="1">
+        <v>3317664</v>
+      </c>
+      <c r="H46" s="1">
+        <v>3330520</v>
+      </c>
+      <c r="I46" s="1">
+        <v>3362016</v>
+      </c>
+      <c r="J46" s="1">
+        <v>3305168</v>
+      </c>
+      <c r="K46" s="1">
+        <v>3341616</v>
+      </c>
+      <c r="L46">
+        <f t="shared" si="0"/>
+        <v>3331396.8</v>
       </c>
     </row>
     <row r="47" spans="5:12" x14ac:dyDescent="0.25">
@@ -1411,14 +1902,24 @@
       <c r="F47" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
-      <c r="I47" s="1"/>
-      <c r="J47" s="1"/>
-      <c r="K47" s="1"/>
-      <c r="L47" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="G47" s="1">
+        <v>960.6</v>
+      </c>
+      <c r="H47" s="1">
+        <v>960.9</v>
+      </c>
+      <c r="I47" s="1">
+        <v>960.7</v>
+      </c>
+      <c r="J47" s="1">
+        <v>960.8</v>
+      </c>
+      <c r="K47" s="1">
+        <v>960.6</v>
+      </c>
+      <c r="L47">
+        <f t="shared" si="0"/>
+        <v>960.72</v>
       </c>
     </row>
     <row r="48" spans="5:12" x14ac:dyDescent="0.25">
@@ -1426,14 +1927,24 @@
       <c r="F48" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
-      <c r="I48" s="1"/>
-      <c r="J48" s="1"/>
-      <c r="K48" s="1"/>
-      <c r="L48" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="G48" s="1">
+        <v>3453.76</v>
+      </c>
+      <c r="H48" s="1">
+        <v>3466.22</v>
+      </c>
+      <c r="I48" s="1">
+        <v>3499.7</v>
+      </c>
+      <c r="J48" s="1">
+        <v>3439.87</v>
+      </c>
+      <c r="K48" s="1">
+        <v>3478.65</v>
+      </c>
+      <c r="L48">
+        <f t="shared" si="0"/>
+        <v>3467.6400000000003</v>
       </c>
     </row>
     <row r="49" spans="5:12" x14ac:dyDescent="0.25">
@@ -1441,11 +1952,21 @@
       <c r="F49" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
-      <c r="I49" s="1"/>
-      <c r="J49" s="1"/>
-      <c r="K49" s="1"/>
+      <c r="G49" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="L49" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -1456,11 +1977,21 @@
       <c r="F50" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G50" s="1"/>
-      <c r="H50" s="1"/>
-      <c r="I50" s="1"/>
-      <c r="J50" s="1"/>
-      <c r="K50" s="1"/>
+      <c r="G50" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="L50" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -1481,8 +2012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E427240-8CAA-40AB-9EE3-C007F0D8C5C2}">
   <dimension ref="E7:L50"/>
   <sheetViews>
-    <sheetView topLeftCell="C28" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41:K50"/>
+    <sheetView topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1492,7 +2023,7 @@
     <col min="7" max="11" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E7" s="3" t="s">
         <v>19</v>
       </c>
@@ -1503,7 +2034,7 @@
       <c r="J7" s="4"/>
       <c r="K7" s="5"/>
     </row>
-    <row r="8" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E8" s="1" t="s">
         <v>0</v>
       </c>
@@ -1526,7 +2057,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E9" s="6">
         <v>100</v>
       </c>
@@ -1549,7 +2080,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E10" s="7"/>
       <c r="F10" s="1" t="s">
         <v>14</v>
@@ -1570,7 +2101,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E11" s="7"/>
       <c r="F11" s="1" t="s">
         <v>15</v>
@@ -1591,7 +2122,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E12" s="7"/>
       <c r="F12" s="1" t="s">
         <v>16</v>
@@ -1612,74 +2143,154 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E13" s="7"/>
       <c r="F13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-    </row>
-    <row r="14" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="G13" s="1">
+        <v>2.7</v>
+      </c>
+      <c r="H13" s="1">
+        <v>2.67</v>
+      </c>
+      <c r="I13" s="1">
+        <v>2.65</v>
+      </c>
+      <c r="J13" s="1">
+        <v>2.67</v>
+      </c>
+      <c r="K13" s="1">
+        <v>2.59</v>
+      </c>
+      <c r="L13">
+        <f>AVERAGE(G13:K13)</f>
+        <v>2.6559999999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E14" s="7"/>
       <c r="F14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-    </row>
-    <row r="15" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="G14" s="1">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0</v>
+      </c>
+      <c r="K14" s="1">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <f t="shared" ref="L14:L50" si="0">AVERAGE(G14:K14)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E15" s="7"/>
       <c r="F15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-    </row>
-    <row r="16" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="G15" s="1">
+        <v>152.85</v>
+      </c>
+      <c r="H15" s="1">
+        <v>44.09</v>
+      </c>
+      <c r="I15" s="1">
+        <v>149.85</v>
+      </c>
+      <c r="J15" s="1">
+        <v>148.1</v>
+      </c>
+      <c r="K15" s="1">
+        <v>148.24</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>128.626</v>
+      </c>
+    </row>
+    <row r="16" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E16" s="7"/>
       <c r="F16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
+      <c r="G16" s="1">
+        <v>3.98</v>
+      </c>
+      <c r="H16" s="1">
+        <v>3.95</v>
+      </c>
+      <c r="I16" s="1">
+        <v>3.89</v>
+      </c>
+      <c r="J16" s="1">
+        <v>3.95</v>
+      </c>
+      <c r="K16" s="1">
+        <v>3.8</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>3.9140000000000001</v>
+      </c>
     </row>
     <row r="17" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E17" s="7"/>
       <c r="F17" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
+      <c r="G17" s="1">
+        <v>4.62</v>
+      </c>
+      <c r="H17" s="1">
+        <v>4.6100000000000003</v>
+      </c>
+      <c r="I17" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="J17" s="1">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="K17" s="1">
+        <v>4.38</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="0"/>
+        <v>4.5419999999999998</v>
+      </c>
     </row>
     <row r="18" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E18" s="7"/>
       <c r="F18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" t="e">
-        <f>AVERAGE(G18:K18)</f>
-        <v>#DIV/0!</v>
+      <c r="G18" s="1">
+        <v>83852</v>
+      </c>
+      <c r="H18" s="1">
+        <v>83852</v>
+      </c>
+      <c r="I18" s="1">
+        <v>83854</v>
+      </c>
+      <c r="J18" s="1">
+        <v>83851</v>
+      </c>
+      <c r="K18" s="1">
+        <v>83858</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="0"/>
+        <v>83853.399999999994</v>
       </c>
     </row>
     <row r="19" spans="5:12" x14ac:dyDescent="0.25">
@@ -1687,14 +2298,24 @@
       <c r="F19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" t="e">
-        <f t="shared" ref="L19:L50" si="0">AVERAGE(G19:K19)</f>
-        <v>#DIV/0!</v>
+      <c r="G19" s="1">
+        <v>961</v>
+      </c>
+      <c r="H19" s="1">
+        <v>960.8</v>
+      </c>
+      <c r="I19" s="1">
+        <v>960</v>
+      </c>
+      <c r="J19" s="1">
+        <v>961</v>
+      </c>
+      <c r="K19" s="1">
+        <v>961</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="0"/>
+        <v>960.76</v>
       </c>
     </row>
     <row r="20" spans="5:12" x14ac:dyDescent="0.25">
@@ -1702,14 +2323,24 @@
       <c r="F20" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="G20" s="1">
+        <v>87.25</v>
+      </c>
+      <c r="H20" s="1">
+        <v>87.27</v>
+      </c>
+      <c r="I20" s="1">
+        <v>87.35</v>
+      </c>
+      <c r="J20" s="1">
+        <v>87.25</v>
+      </c>
+      <c r="K20" s="1">
+        <v>87.26</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="0"/>
+        <v>87.275999999999996</v>
       </c>
     </row>
     <row r="21" spans="5:12" x14ac:dyDescent="0.25">
@@ -1717,11 +2348,21 @@
       <c r="F21" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
+      <c r="G21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="L21" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -1732,11 +2373,21 @@
       <c r="F22" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
+      <c r="G22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="L22" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -1849,14 +2500,24 @@
       <c r="F27" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="G27" s="2">
+        <v>1.76</v>
+      </c>
+      <c r="H27" s="2">
+        <v>1.74</v>
+      </c>
+      <c r="I27" s="2">
+        <v>1.75</v>
+      </c>
+      <c r="J27" s="2">
+        <v>2.27</v>
+      </c>
+      <c r="K27" s="2">
+        <v>2.19</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="0"/>
+        <v>1.9419999999999997</v>
       </c>
     </row>
     <row r="28" spans="5:12" x14ac:dyDescent="0.25">
@@ -1864,14 +2525,24 @@
       <c r="F28" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="G28" s="2">
+        <v>0</v>
+      </c>
+      <c r="H28" s="2">
+        <v>0</v>
+      </c>
+      <c r="I28" s="2">
+        <v>0</v>
+      </c>
+      <c r="J28" s="2">
+        <v>0</v>
+      </c>
+      <c r="K28" s="2">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="5:12" x14ac:dyDescent="0.25">
@@ -1879,14 +2550,24 @@
       <c r="F29" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
-      <c r="L29" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="G29" s="2">
+        <v>149.21</v>
+      </c>
+      <c r="H29" s="2">
+        <v>144.13</v>
+      </c>
+      <c r="I29" s="2">
+        <v>151.38</v>
+      </c>
+      <c r="J29" s="2">
+        <v>72.239999999999995</v>
+      </c>
+      <c r="K29" s="2">
+        <v>150.4</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="0"/>
+        <v>133.47200000000001</v>
       </c>
     </row>
     <row r="30" spans="5:12" x14ac:dyDescent="0.25">
@@ -1894,14 +2575,24 @@
       <c r="F30" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-      <c r="L30" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="G30" s="2">
+        <v>2.6</v>
+      </c>
+      <c r="H30" s="2">
+        <v>2.59</v>
+      </c>
+      <c r="I30" s="2">
+        <v>2.6</v>
+      </c>
+      <c r="J30" s="2">
+        <v>3.62</v>
+      </c>
+      <c r="K30" s="2">
+        <v>3.59</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="5:12" x14ac:dyDescent="0.25">
@@ -1909,14 +2600,24 @@
       <c r="F31" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="G31" s="2">
+        <v>3.08</v>
+      </c>
+      <c r="H31" s="2">
+        <v>3.06</v>
+      </c>
+      <c r="I31" s="2">
+        <v>3.08</v>
+      </c>
+      <c r="J31" s="2">
+        <v>5.15</v>
+      </c>
+      <c r="K31" s="2">
+        <v>4.8099999999999996</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="0"/>
+        <v>3.8359999999999999</v>
       </c>
     </row>
     <row r="32" spans="5:12" x14ac:dyDescent="0.25">
@@ -1924,14 +2625,24 @@
       <c r="F32" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-      <c r="L32" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="G32" s="2">
+        <v>838807</v>
+      </c>
+      <c r="H32" s="2">
+        <v>838807</v>
+      </c>
+      <c r="I32" s="2">
+        <v>838790</v>
+      </c>
+      <c r="J32" s="2">
+        <v>838311</v>
+      </c>
+      <c r="K32" s="2">
+        <v>838384</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="0"/>
+        <v>838619.8</v>
       </c>
     </row>
     <row r="33" spans="5:12" x14ac:dyDescent="0.25">
@@ -1939,14 +2650,24 @@
       <c r="F33" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-      <c r="L33" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="G33" s="2">
+        <v>960.5</v>
+      </c>
+      <c r="H33" s="2">
+        <v>960.5</v>
+      </c>
+      <c r="I33" s="2">
+        <v>960.5</v>
+      </c>
+      <c r="J33" s="2">
+        <v>960.7</v>
+      </c>
+      <c r="K33" s="2">
+        <v>960.6</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="0"/>
+        <v>960.56000000000006</v>
       </c>
     </row>
     <row r="34" spans="5:12" x14ac:dyDescent="0.25">
@@ -1954,14 +2675,24 @@
       <c r="F34" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
-      <c r="L34" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="G34" s="2">
+        <v>873.32</v>
+      </c>
+      <c r="H34" s="2">
+        <v>873.34</v>
+      </c>
+      <c r="I34" s="2">
+        <v>873.31</v>
+      </c>
+      <c r="J34" s="2">
+        <v>872.64</v>
+      </c>
+      <c r="K34" s="2">
+        <v>872.8</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="0"/>
+        <v>873.08199999999999</v>
       </c>
     </row>
     <row r="35" spans="5:12" x14ac:dyDescent="0.25">
@@ -1969,11 +2700,21 @@
       <c r="F35" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
+      <c r="G35" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="L35" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -1984,11 +2725,21 @@
       <c r="F36" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
+      <c r="G36" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="L36" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -2101,14 +2852,24 @@
       <c r="F41" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
-      <c r="K41" s="1"/>
-      <c r="L41" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="G41" s="1">
+        <v>1560</v>
+      </c>
+      <c r="H41" s="1">
+        <v>1580</v>
+      </c>
+      <c r="I41" s="1">
+        <v>1560</v>
+      </c>
+      <c r="J41" s="1">
+        <v>1500</v>
+      </c>
+      <c r="K41" s="1">
+        <v>1520</v>
+      </c>
+      <c r="L41">
+        <f t="shared" si="0"/>
+        <v>1544</v>
       </c>
     </row>
     <row r="42" spans="5:12" x14ac:dyDescent="0.25">
@@ -2116,14 +2877,24 @@
       <c r="F42" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
-      <c r="K42" s="1"/>
-      <c r="L42" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="G42" s="1">
+        <v>0</v>
+      </c>
+      <c r="H42" s="1">
+        <v>0</v>
+      </c>
+      <c r="I42" s="1">
+        <v>0</v>
+      </c>
+      <c r="J42" s="1">
+        <v>0</v>
+      </c>
+      <c r="K42" s="1">
+        <v>0</v>
+      </c>
+      <c r="L42">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="5:12" x14ac:dyDescent="0.25">
@@ -2131,14 +2902,24 @@
       <c r="F43" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
-      <c r="J43" s="1"/>
-      <c r="K43" s="1"/>
-      <c r="L43" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="G43" s="1">
+        <v>2100</v>
+      </c>
+      <c r="H43" s="1">
+        <v>2000</v>
+      </c>
+      <c r="I43" s="1">
+        <v>1990</v>
+      </c>
+      <c r="J43" s="1">
+        <v>1900</v>
+      </c>
+      <c r="K43" s="1">
+        <v>1960</v>
+      </c>
+      <c r="L43">
+        <f t="shared" si="0"/>
+        <v>1990</v>
       </c>
     </row>
     <row r="44" spans="5:12" x14ac:dyDescent="0.25">
@@ -2146,14 +2927,24 @@
       <c r="F44" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
-      <c r="K44" s="1"/>
-      <c r="L44" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="G44" s="1">
+        <v>1820</v>
+      </c>
+      <c r="H44" s="1">
+        <v>1840</v>
+      </c>
+      <c r="I44" s="1">
+        <v>1820</v>
+      </c>
+      <c r="J44" s="1">
+        <v>1750</v>
+      </c>
+      <c r="K44" s="1">
+        <v>1760</v>
+      </c>
+      <c r="L44">
+        <f t="shared" si="0"/>
+        <v>1798</v>
       </c>
     </row>
     <row r="45" spans="5:12" x14ac:dyDescent="0.25">
@@ -2161,14 +2952,24 @@
       <c r="F45" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
-      <c r="I45" s="1"/>
-      <c r="J45" s="1"/>
-      <c r="K45" s="1"/>
-      <c r="L45" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="G45" s="1">
+        <v>1840</v>
+      </c>
+      <c r="H45" s="1">
+        <v>1850</v>
+      </c>
+      <c r="I45" s="1">
+        <v>1830</v>
+      </c>
+      <c r="J45" s="1">
+        <v>1770</v>
+      </c>
+      <c r="K45" s="1">
+        <v>1770</v>
+      </c>
+      <c r="L45">
+        <f t="shared" si="0"/>
+        <v>1812</v>
       </c>
     </row>
     <row r="46" spans="5:12" x14ac:dyDescent="0.25">
@@ -2176,14 +2977,24 @@
       <c r="F46" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
-      <c r="I46" s="1"/>
-      <c r="J46" s="1"/>
-      <c r="K46" s="1"/>
-      <c r="L46" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="G46" s="1">
+        <v>1309204</v>
+      </c>
+      <c r="H46" s="1">
+        <v>1301619</v>
+      </c>
+      <c r="I46" s="1">
+        <v>1310174</v>
+      </c>
+      <c r="J46" s="1">
+        <v>1340088</v>
+      </c>
+      <c r="K46" s="1">
+        <v>1333974</v>
+      </c>
+      <c r="L46">
+        <f t="shared" si="0"/>
+        <v>1319011.8</v>
       </c>
     </row>
     <row r="47" spans="5:12" x14ac:dyDescent="0.25">
@@ -2191,14 +3002,24 @@
       <c r="F47" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
-      <c r="I47" s="1"/>
-      <c r="J47" s="1"/>
-      <c r="K47" s="1"/>
-      <c r="L47" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="G47" s="1">
+        <v>960.8</v>
+      </c>
+      <c r="H47" s="1">
+        <v>961</v>
+      </c>
+      <c r="I47" s="1">
+        <v>960.8</v>
+      </c>
+      <c r="J47" s="1">
+        <v>960.6</v>
+      </c>
+      <c r="K47" s="1">
+        <v>960.9</v>
+      </c>
+      <c r="L47">
+        <f t="shared" si="0"/>
+        <v>960.81999999999994</v>
       </c>
     </row>
     <row r="48" spans="5:12" x14ac:dyDescent="0.25">
@@ -2206,14 +3027,24 @@
       <c r="F48" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
-      <c r="I48" s="1"/>
-      <c r="J48" s="1"/>
-      <c r="K48" s="1"/>
-      <c r="L48" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="G48" s="1">
+        <v>1362.58</v>
+      </c>
+      <c r="H48" s="1">
+        <v>1354.46</v>
+      </c>
+      <c r="I48" s="1">
+        <v>1363.64</v>
+      </c>
+      <c r="J48" s="1">
+        <v>1395.11</v>
+      </c>
+      <c r="K48" s="1">
+        <v>1388.2</v>
+      </c>
+      <c r="L48">
+        <f t="shared" si="0"/>
+        <v>1372.798</v>
       </c>
     </row>
     <row r="49" spans="5:12" x14ac:dyDescent="0.25">
@@ -2221,11 +3052,21 @@
       <c r="F49" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
-      <c r="I49" s="1"/>
-      <c r="J49" s="1"/>
-      <c r="K49" s="1"/>
+      <c r="G49" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="L49" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -2236,11 +3077,21 @@
       <c r="F50" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G50" s="1"/>
-      <c r="H50" s="1"/>
-      <c r="I50" s="1"/>
-      <c r="J50" s="1"/>
-      <c r="K50" s="1"/>
+      <c r="G50" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="L50" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -4602,10 +5453,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{491B2463-697C-4FC5-A88C-76F5DBC70B85}">
-  <dimension ref="E7:L50"/>
+  <dimension ref="E7:L51"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I50" sqref="I50"/>
+    <sheetView topLeftCell="B25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13:L51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4613,6 +5464,7 @@
     <col min="5" max="5" width="33.7109375" customWidth="1"/>
     <col min="6" max="6" width="32.5703125" customWidth="1"/>
     <col min="7" max="11" width="10" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="7" spans="5:12" x14ac:dyDescent="0.25">
@@ -4773,7 +5625,7 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14">
-        <f t="shared" ref="L14:L50" si="0">AVERAGE(G14:I14)</f>
+        <f t="shared" ref="L14:L51" si="0">AVERAGE(G14:I14)</f>
         <v>0</v>
       </c>
     </row>
@@ -5565,6 +6417,12 @@
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
       <c r="L50" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="51" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="L51" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -5585,8 +6443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FB6DA92-7223-446A-BEE3-0FF2B848B2A6}">
   <dimension ref="E7:L50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D26" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N41" sqref="N41"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>